<commit_message>
comments and the todo's are done.
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
@@ -1787,16 +1787,76 @@
     </row>
     <row r="96">
       <c r="A96" s="3" t="n">
-        <v>44838.99697754191</v>
-      </c>
-      <c r="B96" t="inlineStr">
+        <v>44838.9969775463</v>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
         <is>
           <t>AÇIK</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>4.7</t>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="n">
+        <v>44839.02611079861</v>
+      </c>
+      <c r="B97" s="2" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>Sistem Kapalı</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="n">
+        <v>44839.0261312037</v>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="n">
+        <v>44839.02615079861</v>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="n">
+        <v>44839.02616507</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Sistem Kapalı</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
I am gonna test the request for the real life. Gonna see if they are gonna susoend us or not. The test is gonna be fot 8 hours.
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
@@ -1847,16 +1847,31 @@
     </row>
     <row r="100">
       <c r="A100" s="3" t="n">
-        <v>44839.02616507</v>
-      </c>
-      <c r="B100" t="inlineStr">
+        <v>44839.02616506944</v>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
         <is>
           <t>KAPALI</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="C100" s="2" t="inlineStr">
         <is>
           <t>Sistem Kapalı</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="n">
+        <v>44839.03433370872</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>4.6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
OPEN/CLOSE Status is not clear now, we have to test it with the real case
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -111,7 +111,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -132,16 +132,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.79"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -154,6 +158,24 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
loop is working fine, all the restaurants are signed in, waiting for the table design so that I write the data to the table accoring to that
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -453,11 +453,11 @@
     <row r="1">
       <c r="A1" s="0" t="inlineStr">
         <is>
-          <t>konoha-bagdat-cad-kadikoy-istanbul</t>
+          <t>alle-bowls-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B1" s="1" t="n">
-        <v>44839.80821994213</v>
+        <v>44841.50505825232</v>
       </c>
       <c r="C1" s="0" t="inlineStr">
         <is>
@@ -466,58 +466,58 @@
       </c>
       <c r="D1" s="0" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>cosa-bi-corba-bi-salata-kozyatagi-mah-kadikoy-istanbul</t>
+          <t>ariana-s-cheesecake-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>44839.80822732639</v>
+        <v>44841.50512471065</v>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>AÇIK</t>
+          <t>KAPALI</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>giresun-konagi-restoran-bagcilar-istanbul</t>
+          <t>restoran</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>44839.80823481482</v>
+        <v>44841.50520675926</v>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>KAPALI</t>
+          <t>AÇIK</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>NO RATING</t>
+          <t>4.3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>gurme-lahmacun-pide-sahrayicedit-mah-kadikoy-istanbul</t>
+          <t>restoran</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>44839.80823822917</v>
+        <v>44841.50527828703</v>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
@@ -533,11 +533,11 @@
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>konoha-bagdat-cad-kadikoy-istanbul</t>
+          <t>alle-bowls-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>44839.80825618056</v>
+        <v>44841.50718738426</v>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
@@ -546,78 +546,78 @@
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>cosa-bi-corba-bi-salata-kozyatagi-mah-kadikoy-istanbul</t>
+          <t>ariana-s-cheesecake-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>44839.80826113426</v>
+        <v>44841.50726765046</v>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>AÇIK</t>
+          <t>KAPALI</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>giresun-konagi-restoran-bagcilar-istanbul</t>
+          <t>alle-bowls-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>44839.80826431713</v>
+        <v>44841.51303667824</v>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>KAPALI</t>
+          <t>AÇIK</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>NO RATING</t>
+          <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>gurme-lahmacun-pide-sahrayicedit-mah-kadikoy-istanbul</t>
+          <t>ariana-s-cheesecake-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>44839.80826783565</v>
+        <v>44841.51311502315</v>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>AÇIK</t>
+          <t>KAPALI</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>konoha-bagdat-cad-kadikoy-istanbul</t>
+          <t>restoran</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>44839.83417875</v>
+        <v>44841.51319752315</v>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
@@ -626,18 +626,18 @@
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>cosa-bi-corba-bi-salata-kozyatagi-mah-kadikoy-istanbul</t>
+          <t>restoran</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>44839.83418702547</v>
+        <v>44841.51327284722</v>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
@@ -646,127 +646,287 @@
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.6</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>giresun-konagi-restoran-bagcilar-istanbul</t>
+          <t>cosa-bi-corba-bi-salata-acibadem-mah-kadikoy-istanbul</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>44839.83419753472</v>
+        <v>44841.51334820602</v>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>KAPALI</t>
+          <t>AÇIK</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>NO RATING</t>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>gurme-lahmacun-pide-sahrayicedit-mah-kadikoy-istanbul</t>
+          <t>restoran</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>44839.83420465278</v>
+        <v>44841.51343730324</v>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>AÇIK</t>
+          <t>KAPALI</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="inlineStr">
+        <is>
+          <t>restoran</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>44841.51351729166</v>
+      </c>
+      <c r="C13" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="inlineStr">
+        <is>
+          <t>doyuyo-sarayardi-cad-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>44841.51360233796</v>
+      </c>
+      <c r="C14" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="inlineStr">
+        <is>
+          <t>el-pollo-lasso-acibadem-mah-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>44841.51368598379</v>
+      </c>
+      <c r="C15" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="inlineStr">
+        <is>
+          <t>alle-bowls-acibadem-mah-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>44841.51379228009</v>
+      </c>
+      <c r="C16" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="inlineStr">
+        <is>
+          <t>ariana-s-cheesecake-acibadem-mah-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>44841.51386959491</v>
+      </c>
+      <c r="C17" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="inlineStr">
+        <is>
+          <t>alle-bowls-acibadem-mah-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>44841.51410226852</v>
+      </c>
+      <c r="C18" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="inlineStr">
+        <is>
+          <t>ariana-s-cheesecake-acibadem-mah-kadikoy-istanbul</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>44841.51416706019</v>
+      </c>
+      <c r="C19" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="inlineStr">
+        <is>
+          <t>restoran</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>44841.51423962963</v>
+      </c>
+      <c r="C20" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="inlineStr">
+        <is>
+          <t>restoran</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>44841.51431548611</v>
+      </c>
+      <c r="C21" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
           <t>4.6</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>konoha-bagdat-cad-kadikoy-istanbul</t>
-        </is>
-      </c>
-      <c r="B13" s="1" t="n">
-        <v>44839.8342205937</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>AÇIK</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>4.7</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>cosa-bi-corba-bi-salata-kozyatagi-mah-kadikoy-istanbul</t>
-        </is>
-      </c>
-      <c r="B14" s="1" t="n">
-        <v>44839.83422474632</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>AÇIK</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>44841.51753185411</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
         <is>
           <t>4.4</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>giresun-konagi-restoran-bagcilar-istanbul</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>44839.8342283618</v>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>44841.51761353836</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>KAPALI</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>NO RATING</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>gurme-lahmacun-pide-sahrayicedit-mah-kadikoy-istanbul</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>44839.83423231573</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>AÇIK</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>4.6</t>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>44841.51770283478</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>4.3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
there is some percatange of failure but the app keeps working and bypass it. Gonna test that if the app gives the same errors for the same url over and over again
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -442,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D350"/>
+  <dimension ref="A1:D512"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -7411,42 +7411,3282 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" t="inlineStr">
+      <c r="A349" s="0" t="inlineStr">
         <is>
           <t>Acıbadem Alle Bowls</t>
         </is>
       </c>
       <c r="B349" s="1" t="n">
-        <v>44843.03623266301</v>
-      </c>
-      <c r="C349" t="inlineStr">
-        <is>
-          <t>AÇIK</t>
-        </is>
-      </c>
-      <c r="D349" t="inlineStr">
+        <v>44843.03623266204</v>
+      </c>
+      <c r="C349" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D349" s="0" t="inlineStr">
         <is>
           <t>4.4</t>
         </is>
       </c>
     </row>
     <row r="350">
-      <c r="A350" t="inlineStr">
+      <c r="A350" s="0" t="inlineStr">
         <is>
           <t>Acıbadem Arianas Cheesecake</t>
         </is>
       </c>
       <c r="B350" s="1" t="n">
-        <v>44843.03629944244</v>
-      </c>
-      <c r="C350" t="inlineStr">
-        <is>
-          <t>KAPALI</t>
-        </is>
-      </c>
-      <c r="D350" t="inlineStr">
+        <v>44843.03629944444</v>
+      </c>
+      <c r="C350" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D350" s="0" t="inlineStr">
         <is>
           <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B351" s="1" t="n">
+        <v>44843.03831399306</v>
+      </c>
+      <c r="C351" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D351" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B352" s="1" t="n">
+        <v>44843.03837776621</v>
+      </c>
+      <c r="C352" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D352" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B353" s="1" t="n">
+        <v>44843.0384467824</v>
+      </c>
+      <c r="C353" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D353" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B354" s="1" t="n">
+        <v>44843.03852373843</v>
+      </c>
+      <c r="C354" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D354" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Çosa</t>
+        </is>
+      </c>
+      <c r="B355" s="1" t="n">
+        <v>44843.0385958449</v>
+      </c>
+      <c r="C355" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D355" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B356" s="1" t="n">
+        <v>44843.03866386574</v>
+      </c>
+      <c r="C356" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D356" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B357" s="1" t="n">
+        <v>44843.03873115741</v>
+      </c>
+      <c r="C357" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D357" s="0" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Doyuyo</t>
+        </is>
+      </c>
+      <c r="B358" s="1" t="n">
+        <v>44843.0388</v>
+      </c>
+      <c r="C358" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D358" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B359" s="1" t="n">
+        <v>44843.03886686343</v>
+      </c>
+      <c r="C359" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D359" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Etişler Köfte</t>
+        </is>
+      </c>
+      <c r="B360" s="1" t="n">
+        <v>44843.0389340162</v>
+      </c>
+      <c r="C360" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D360" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Fadelini</t>
+        </is>
+      </c>
+      <c r="B361" s="1" t="n">
+        <v>44843.03899912037</v>
+      </c>
+      <c r="C361" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D361" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B362" s="1" t="n">
+        <v>44843.03907046296</v>
+      </c>
+      <c r="C362" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D362" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem G&amp;G Burger</t>
+        </is>
+      </c>
+      <c r="B363" s="1" t="n">
+        <v>44843.03914486111</v>
+      </c>
+      <c r="C363" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D363" s="0" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B364" s="1" t="n">
+        <v>44843.03921504629</v>
+      </c>
+      <c r="C364" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D364" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Jay Jay Fries</t>
+        </is>
+      </c>
+      <c r="B365" s="1" t="n">
+        <v>44843.03928465278</v>
+      </c>
+      <c r="C365" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D365" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Kale Arkası Mutfak</t>
+        </is>
+      </c>
+      <c r="B366" s="1" t="n">
+        <v>44843.03935349537</v>
+      </c>
+      <c r="C366" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D366" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B367" s="1" t="n">
+        <v>44843.03942228009</v>
+      </c>
+      <c r="C367" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D367" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Madritas</t>
+        </is>
+      </c>
+      <c r="B368" s="1" t="n">
+        <v>44843.03948981482</v>
+      </c>
+      <c r="C368" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D368" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B369" s="1" t="n">
+        <v>44843.03956107639</v>
+      </c>
+      <c r="C369" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D369" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B370" s="1" t="n">
+        <v>44843.03963002315</v>
+      </c>
+      <c r="C370" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D370" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Noody</t>
+        </is>
+      </c>
+      <c r="B371" s="1" t="n">
+        <v>44843.03969864584</v>
+      </c>
+      <c r="C371" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D371" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Red Haag</t>
+        </is>
+      </c>
+      <c r="B372" s="1" t="n">
+        <v>44843.03976865741</v>
+      </c>
+      <c r="C372" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D372" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B373" s="1" t="n">
+        <v>44843.03983612268</v>
+      </c>
+      <c r="C373" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D373" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Seez Beez</t>
+        </is>
+      </c>
+      <c r="B374" s="1" t="n">
+        <v>44843.03990484954</v>
+      </c>
+      <c r="C374" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D374" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B375" s="1" t="n">
+        <v>44843.03997587963</v>
+      </c>
+      <c r="C375" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D375" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Tabur Köfte</t>
+        </is>
+      </c>
+      <c r="B376" s="1" t="n">
+        <v>44843.04004670139</v>
+      </c>
+      <c r="C376" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D376" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem The Bowl</t>
+        </is>
+      </c>
+      <c r="B377" s="1" t="n">
+        <v>44843.04011321759</v>
+      </c>
+      <c r="C377" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D377" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="0" t="inlineStr">
+        <is>
+          <t>Acıbadem Veganista</t>
+        </is>
+      </c>
+      <c r="B378" s="1" t="n">
+        <v>44843.04018099537</v>
+      </c>
+      <c r="C378" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D378" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B379" s="1" t="n">
+        <v>44843.04024497685</v>
+      </c>
+      <c r="C379" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D379" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B380" s="1" t="n">
+        <v>44843.04031466435</v>
+      </c>
+      <c r="C380" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D380" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B381" s="1" t="n">
+        <v>44843.04038197917</v>
+      </c>
+      <c r="C381" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D381" s="0" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B382" s="1" t="n">
+        <v>44843.04045106481</v>
+      </c>
+      <c r="C382" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D382" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="0" t="inlineStr">
+        <is>
+          <t>Ataşhir Çosa</t>
+        </is>
+      </c>
+      <c r="B383" s="1" t="n">
+        <v>44843.04052128473</v>
+      </c>
+      <c r="C383" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D383" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B384" s="1" t="n">
+        <v>44843.04059241898</v>
+      </c>
+      <c r="C384" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D384" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B385" s="1" t="n">
+        <v>44843.04065925926</v>
+      </c>
+      <c r="C385" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D385" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Doyuyo</t>
+        </is>
+      </c>
+      <c r="B386" s="1" t="n">
+        <v>44843.04072699074</v>
+      </c>
+      <c r="C386" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D386" s="0" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B387" s="1" t="n">
+        <v>44843.04079577547</v>
+      </c>
+      <c r="C387" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D387" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Fadelini</t>
+        </is>
+      </c>
+      <c r="B388" s="1" t="n">
+        <v>44843.04086320602</v>
+      </c>
+      <c r="C388" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D388" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B389" s="1" t="n">
+        <v>44843.04093238426</v>
+      </c>
+      <c r="C389" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D389" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B390" s="1" t="n">
+        <v>44843.04100114583</v>
+      </c>
+      <c r="C390" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D390" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Jay Jay Fries</t>
+        </is>
+      </c>
+      <c r="B391" s="1" t="n">
+        <v>44843.04106991898</v>
+      </c>
+      <c r="C391" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D391" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Kale Arkası Mutfak</t>
+        </is>
+      </c>
+      <c r="B392" s="1" t="n">
+        <v>44843.04113962963</v>
+      </c>
+      <c r="C392" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D392" s="0" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B393" s="1" t="n">
+        <v>44843.04121071759</v>
+      </c>
+      <c r="C393" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D393" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Madritas</t>
+        </is>
+      </c>
+      <c r="B394" s="1" t="n">
+        <v>44843.04127703704</v>
+      </c>
+      <c r="C394" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D394" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B395" s="1" t="n">
+        <v>44843.04134708333</v>
+      </c>
+      <c r="C395" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D395" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B396" s="1" t="n">
+        <v>44843.04141603009</v>
+      </c>
+      <c r="C396" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D396" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Noody</t>
+        </is>
+      </c>
+      <c r="B397" s="1" t="n">
+        <v>44843.04148467592</v>
+      </c>
+      <c r="C397" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D397" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Red Haag</t>
+        </is>
+      </c>
+      <c r="B398" s="1" t="n">
+        <v>44843.04155229167</v>
+      </c>
+      <c r="C398" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D398" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B399" s="1" t="n">
+        <v>44843.0416209375</v>
+      </c>
+      <c r="C399" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D399" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Seez Beez</t>
+        </is>
+      </c>
+      <c r="B400" s="1" t="n">
+        <v>44843.04168976852</v>
+      </c>
+      <c r="C400" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D400" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B401" s="1" t="n">
+        <v>44843.04175962963</v>
+      </c>
+      <c r="C401" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D401" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Sushi Master</t>
+        </is>
+      </c>
+      <c r="B402" s="1" t="n">
+        <v>44843.04182846065</v>
+      </c>
+      <c r="C402" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D402" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir The Bowl</t>
+        </is>
+      </c>
+      <c r="B403" s="1" t="n">
+        <v>44843.04189815972</v>
+      </c>
+      <c r="C403" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D403" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0" t="inlineStr">
+        <is>
+          <t>Ataşehir Veganista</t>
+        </is>
+      </c>
+      <c r="B404" s="1" t="n">
+        <v>44843.04196712963</v>
+      </c>
+      <c r="C404" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D404" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B405" s="1" t="n">
+        <v>44843.04204189814</v>
+      </c>
+      <c r="C405" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D405" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B406" s="1" t="n">
+        <v>44843.04211018518</v>
+      </c>
+      <c r="C406" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D406" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B407" s="1" t="n">
+        <v>44843.0421774537</v>
+      </c>
+      <c r="C407" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D407" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B408" s="1" t="n">
+        <v>44843.04224534722</v>
+      </c>
+      <c r="C408" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D408" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Çosa</t>
+        </is>
+      </c>
+      <c r="B409" s="1" t="n">
+        <v>44843.0423143287</v>
+      </c>
+      <c r="C409" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D409" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B410" s="1" t="n">
+        <v>44843.0423830787</v>
+      </c>
+      <c r="C410" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D410" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B411" s="1" t="n">
+        <v>44843.0424515162</v>
+      </c>
+      <c r="C411" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D411" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Doyuyo</t>
+        </is>
+      </c>
+      <c r="B412" s="1" t="n">
+        <v>44843.04251814815</v>
+      </c>
+      <c r="C412" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D412" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B413" s="1" t="n">
+        <v>44843.04258814815</v>
+      </c>
+      <c r="C413" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D413" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Etişler Köfte</t>
+        </is>
+      </c>
+      <c r="B414" s="1" t="n">
+        <v>44843.04265788195</v>
+      </c>
+      <c r="C414" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D414" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Fadelini</t>
+        </is>
+      </c>
+      <c r="B415" s="1" t="n">
+        <v>44843.04272659722</v>
+      </c>
+      <c r="C415" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D415" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B416" s="1" t="n">
+        <v>44843.04279984954</v>
+      </c>
+      <c r="C416" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D416" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı G&amp;G Burger</t>
+        </is>
+      </c>
+      <c r="B417" s="1" t="n">
+        <v>44843.04287116898</v>
+      </c>
+      <c r="C417" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D417" s="0" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B418" s="1" t="n">
+        <v>44843.04294013889</v>
+      </c>
+      <c r="C418" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D418" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Jay Jay Fries</t>
+        </is>
+      </c>
+      <c r="B419" s="1" t="n">
+        <v>44843.04301006944</v>
+      </c>
+      <c r="C419" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D419" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Kale Arkası Mutfak</t>
+        </is>
+      </c>
+      <c r="B420" s="1" t="n">
+        <v>44843.04307866898</v>
+      </c>
+      <c r="C420" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D420" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B421" s="1" t="n">
+        <v>44843.04314688657</v>
+      </c>
+      <c r="C421" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D421" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Madritas</t>
+        </is>
+      </c>
+      <c r="B422" s="1" t="n">
+        <v>44843.0432162963</v>
+      </c>
+      <c r="C422" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D422" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B423" s="1" t="n">
+        <v>44843.04328482639</v>
+      </c>
+      <c r="C423" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D423" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B424" s="1" t="n">
+        <v>44843.0433574074</v>
+      </c>
+      <c r="C424" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D424" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Noody</t>
+        </is>
+      </c>
+      <c r="B425" s="1" t="n">
+        <v>44843.04342721065</v>
+      </c>
+      <c r="C425" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D425" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Red Haag</t>
+        </is>
+      </c>
+      <c r="B426" s="1" t="n">
+        <v>44843.04349601852</v>
+      </c>
+      <c r="C426" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D426" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B427" s="1" t="n">
+        <v>44843.04356371528</v>
+      </c>
+      <c r="C427" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D427" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B428" s="1" t="n">
+        <v>44843.0436346875</v>
+      </c>
+      <c r="C428" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D428" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Sushi Master</t>
+        </is>
+      </c>
+      <c r="B429" s="1" t="n">
+        <v>44843.04370210648</v>
+      </c>
+      <c r="C429" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D429" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Tabur Köfte</t>
+        </is>
+      </c>
+      <c r="B430" s="1" t="n">
+        <v>44843.04377052083</v>
+      </c>
+      <c r="C430" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D430" s="0" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı The Bowl</t>
+        </is>
+      </c>
+      <c r="B431" s="1" t="n">
+        <v>44843.0438384838</v>
+      </c>
+      <c r="C431" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D431" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="inlineStr">
+        <is>
+          <t>Kozyatağı Veganista</t>
+        </is>
+      </c>
+      <c r="B432" s="1" t="n">
+        <v>44843.04390849537</v>
+      </c>
+      <c r="C432" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D432" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="inlineStr">
+        <is>
+          <t>FSM Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B433" s="1" t="n">
+        <v>44843.04397665509</v>
+      </c>
+      <c r="C433" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D433" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="inlineStr">
+        <is>
+          <t>FSM Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B434" s="1" t="n">
+        <v>44843.04404233796</v>
+      </c>
+      <c r="C434" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D434" s="0" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="inlineStr">
+        <is>
+          <t>FSM Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B435" s="1" t="n">
+        <v>44843.04410719907</v>
+      </c>
+      <c r="C435" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D435" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="inlineStr">
+        <is>
+          <t>FSM Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B436" s="1" t="n">
+        <v>44843.04417447917</v>
+      </c>
+      <c r="C436" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D436" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="inlineStr">
+        <is>
+          <t>FSM Çosa</t>
+        </is>
+      </c>
+      <c r="B437" s="1" t="n">
+        <v>44843.04424515046</v>
+      </c>
+      <c r="C437" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D437" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="inlineStr">
+        <is>
+          <t>FSM Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B438" s="1" t="n">
+        <v>44843.04431381945</v>
+      </c>
+      <c r="C438" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D438" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="inlineStr">
+        <is>
+          <t>FSM Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B439" s="1" t="n">
+        <v>44843.04438068287</v>
+      </c>
+      <c r="C439" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D439" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="inlineStr">
+        <is>
+          <t>FSM El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B440" s="1" t="n">
+        <v>44843.04445349537</v>
+      </c>
+      <c r="C440" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D440" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="inlineStr">
+        <is>
+          <t>FSM Etişler Köfte</t>
+        </is>
+      </c>
+      <c r="B441" s="1" t="n">
+        <v>44843.04452459491</v>
+      </c>
+      <c r="C441" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D441" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="inlineStr">
+        <is>
+          <t>FSM Fadelini</t>
+        </is>
+      </c>
+      <c r="B442" s="1" t="n">
+        <v>44843.04459060185</v>
+      </c>
+      <c r="C442" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D442" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="inlineStr">
+        <is>
+          <t>FSM Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B443" s="1" t="n">
+        <v>44843.04465982639</v>
+      </c>
+      <c r="C443" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D443" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="inlineStr">
+        <is>
+          <t>FSM G&amp;G Burger</t>
+        </is>
+      </c>
+      <c r="B444" s="1" t="n">
+        <v>44843.04472878472</v>
+      </c>
+      <c r="C444" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D444" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="inlineStr">
+        <is>
+          <t>FSM Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B445" s="1" t="n">
+        <v>44843.04479969908</v>
+      </c>
+      <c r="C445" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D445" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="inlineStr">
+        <is>
+          <t>FSM Kale Arkası Mutfak</t>
+        </is>
+      </c>
+      <c r="B446" s="1" t="n">
+        <v>44843.04486822917</v>
+      </c>
+      <c r="C446" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D446" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="inlineStr">
+        <is>
+          <t>FSM Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B447" s="1" t="n">
+        <v>44843.04493694445</v>
+      </c>
+      <c r="C447" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D447" s="0" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="inlineStr">
+        <is>
+          <t>FSM Madritas</t>
+        </is>
+      </c>
+      <c r="B448" s="1" t="n">
+        <v>44843.04500339121</v>
+      </c>
+      <c r="C448" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D448" s="0" t="inlineStr">
+        <is>
+          <t>4.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="inlineStr">
+        <is>
+          <t>FSM Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B449" s="1" t="n">
+        <v>44843.04507107639</v>
+      </c>
+      <c r="C449" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D449" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="inlineStr">
+        <is>
+          <t>FSM Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B450" s="1" t="n">
+        <v>44843.0451434838</v>
+      </c>
+      <c r="C450" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D450" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="inlineStr">
+        <is>
+          <t>FSM Noody</t>
+        </is>
+      </c>
+      <c r="B451" s="1" t="n">
+        <v>44843.04521217592</v>
+      </c>
+      <c r="C451" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D451" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="inlineStr">
+        <is>
+          <t>FSM Red Haag</t>
+        </is>
+      </c>
+      <c r="B452" s="1" t="n">
+        <v>44843.04528092593</v>
+      </c>
+      <c r="C452" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D452" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="inlineStr">
+        <is>
+          <t>FSM Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B453" s="1" t="n">
+        <v>44843.04534928241</v>
+      </c>
+      <c r="C453" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D453" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="inlineStr">
+        <is>
+          <t>FSM Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B454" s="1" t="n">
+        <v>44843.04542016204</v>
+      </c>
+      <c r="C454" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D454" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="inlineStr">
+        <is>
+          <t>FSM Tabur Köfte</t>
+        </is>
+      </c>
+      <c r="B455" s="1" t="n">
+        <v>44843.04549662037</v>
+      </c>
+      <c r="C455" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D455" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="inlineStr">
+        <is>
+          <t>FSM The Bowl</t>
+        </is>
+      </c>
+      <c r="B456" s="1" t="n">
+        <v>44843.04556526621</v>
+      </c>
+      <c r="C456" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D456" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="inlineStr">
+        <is>
+          <t>FSM Veganista</t>
+        </is>
+      </c>
+      <c r="B457" s="1" t="n">
+        <v>44843.04563414352</v>
+      </c>
+      <c r="C457" s="0" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D457" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B458" s="1" t="n">
+        <v>44843.0457010301</v>
+      </c>
+      <c r="C458" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D458" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B459" s="1" t="n">
+        <v>44843.04576777778</v>
+      </c>
+      <c r="C459" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D459" s="0" t="inlineStr">
+        <is>
+          <t>3.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B460" s="1" t="n">
+        <v>44843.04583372685</v>
+      </c>
+      <c r="C460" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D460" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B461" s="1" t="n">
+        <v>44843.04590192129</v>
+      </c>
+      <c r="C461" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D461" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Çosa</t>
+        </is>
+      </c>
+      <c r="B462" s="1" t="n">
+        <v>44843.04596954861</v>
+      </c>
+      <c r="C462" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D462" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B463" s="1" t="n">
+        <v>44843.04604407407</v>
+      </c>
+      <c r="C463" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D463" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B464" s="1" t="n">
+        <v>44843.04610972222</v>
+      </c>
+      <c r="C464" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D464" s="0" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="inlineStr">
+        <is>
+          <t>Maslak El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B465" s="1" t="n">
+        <v>44843.04617675926</v>
+      </c>
+      <c r="C465" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D465" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Etişler Köfte</t>
+        </is>
+      </c>
+      <c r="B466" s="1" t="n">
+        <v>44843.04624313657</v>
+      </c>
+      <c r="C466" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D466" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Fadelini</t>
+        </is>
+      </c>
+      <c r="B467" s="1" t="n">
+        <v>44843.04630910879</v>
+      </c>
+      <c r="C467" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D467" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B468" s="1" t="n">
+        <v>44843.04637792824</v>
+      </c>
+      <c r="C468" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D468" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="inlineStr">
+        <is>
+          <t>Maslak G&amp;G Burger</t>
+        </is>
+      </c>
+      <c r="B469" s="1" t="n">
+        <v>44843.04644815972</v>
+      </c>
+      <c r="C469" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D469" s="0" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B470" s="1" t="n">
+        <v>44843.04651694444</v>
+      </c>
+      <c r="C470" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D470" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Jay Jay Fries</t>
+        </is>
+      </c>
+      <c r="B471" s="1" t="n">
+        <v>44843.04658453703</v>
+      </c>
+      <c r="C471" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D471" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Kale Arkası Mutfak</t>
+        </is>
+      </c>
+      <c r="B472" s="1" t="n">
+        <v>44843.04665197917</v>
+      </c>
+      <c r="C472" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D472" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B473" s="1" t="n">
+        <v>44843.04672186343</v>
+      </c>
+      <c r="C473" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D473" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Madritas</t>
+        </is>
+      </c>
+      <c r="B474" s="1" t="n">
+        <v>44843.04678952546</v>
+      </c>
+      <c r="C474" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D474" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B475" s="1" t="n">
+        <v>44843.04685892361</v>
+      </c>
+      <c r="C475" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D475" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B476" s="1" t="n">
+        <v>44843.04692803241</v>
+      </c>
+      <c r="C476" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D476" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Noody</t>
+        </is>
+      </c>
+      <c r="B477" s="1" t="n">
+        <v>44843.04699575232</v>
+      </c>
+      <c r="C477" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D477" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Red Haag</t>
+        </is>
+      </c>
+      <c r="B478" s="1" t="n">
+        <v>44843.04706337963</v>
+      </c>
+      <c r="C478" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D478" s="0" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B479" s="1" t="n">
+        <v>44843.04714746528</v>
+      </c>
+      <c r="C479" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D479" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B480" s="1" t="n">
+        <v>44843.04721497685</v>
+      </c>
+      <c r="C480" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D480" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Sushi Master</t>
+        </is>
+      </c>
+      <c r="B481" s="1" t="n">
+        <v>44843.04728378472</v>
+      </c>
+      <c r="C481" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D481" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Tabur Köfte</t>
+        </is>
+      </c>
+      <c r="B482" s="1" t="n">
+        <v>44843.04735133102</v>
+      </c>
+      <c r="C482" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D482" s="0" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="inlineStr">
+        <is>
+          <t>Maslak The Bowl</t>
+        </is>
+      </c>
+      <c r="B483" s="1" t="n">
+        <v>44843.04742125</v>
+      </c>
+      <c r="C483" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D483" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="inlineStr">
+        <is>
+          <t>Maslak Veganista</t>
+        </is>
+      </c>
+      <c r="B484" s="1" t="n">
+        <v>44843.04749241898</v>
+      </c>
+      <c r="C484" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D484" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B485" s="1" t="n">
+        <v>44843.04755918981</v>
+      </c>
+      <c r="C485" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D485" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B486" s="1" t="n">
+        <v>44843.04763454861</v>
+      </c>
+      <c r="C486" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D486" s="0" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B487" s="1" t="n">
+        <v>44843.04770320602</v>
+      </c>
+      <c r="C487" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D487" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Çosa</t>
+        </is>
+      </c>
+      <c r="B488" s="1" t="n">
+        <v>44843.04777229167</v>
+      </c>
+      <c r="C488" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D488" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="0" t="inlineStr">
+        <is>
+          <t>İzmir El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B489" s="1" t="n">
+        <v>44843.04783844907</v>
+      </c>
+      <c r="C489" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D489" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Fadelini</t>
+        </is>
+      </c>
+      <c r="B490" s="1" t="n">
+        <v>44843.04791307871</v>
+      </c>
+      <c r="C490" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D490" s="0" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Fun For Fit</t>
+        </is>
+      </c>
+      <c r="B491" s="1" t="n">
+        <v>44843.04797950231</v>
+      </c>
+      <c r="C491" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D491" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Gurra Tavuk</t>
+        </is>
+      </c>
+      <c r="B492" s="1" t="n">
+        <v>44843.04804888889</v>
+      </c>
+      <c r="C492" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D492" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Jay Jay Fries</t>
+        </is>
+      </c>
+      <c r="B493" s="1" t="n">
+        <v>44843.048116875</v>
+      </c>
+      <c r="C493" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D493" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Kengeres Çiğ Köfte</t>
+        </is>
+      </c>
+      <c r="B494" s="1" t="n">
+        <v>44843.04820340278</v>
+      </c>
+      <c r="C494" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D494" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Mztps Meze</t>
+        </is>
+      </c>
+      <c r="B495" s="1" t="n">
+        <v>44843.04827916667</v>
+      </c>
+      <c r="C495" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D495" s="0" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Nane Mantı</t>
+        </is>
+      </c>
+      <c r="B496" s="1" t="n">
+        <v>44843.04834690972</v>
+      </c>
+      <c r="C496" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D496" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Noody</t>
+        </is>
+      </c>
+      <c r="B497" s="1" t="n">
+        <v>44843.04841435186</v>
+      </c>
+      <c r="C497" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D497" s="0" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Red Haag</t>
+        </is>
+      </c>
+      <c r="B498" s="1" t="n">
+        <v>44843.04848123842</v>
+      </c>
+      <c r="C498" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D498" s="0" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Rylee's Ranch Salad</t>
+        </is>
+      </c>
+      <c r="B499" s="1" t="n">
+        <v>44843.04854938657</v>
+      </c>
+      <c r="C499" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D499" s="0" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Seez Beez</t>
+        </is>
+      </c>
+      <c r="B500" s="1" t="n">
+        <v>44843.0486169213</v>
+      </c>
+      <c r="C500" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D500" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Senor Torreon</t>
+        </is>
+      </c>
+      <c r="B501" s="1" t="n">
+        <v>44843.04868462963</v>
+      </c>
+      <c r="C501" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D501" s="0" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="0" t="inlineStr">
+        <is>
+          <t>İzmir The Bowl</t>
+        </is>
+      </c>
+      <c r="B502" s="1" t="n">
+        <v>44843.0487625926</v>
+      </c>
+      <c r="C502" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D502" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="0" t="inlineStr">
+        <is>
+          <t>İzmir Veganista</t>
+        </is>
+      </c>
+      <c r="B503" s="1" t="n">
+        <v>44843.0488303588</v>
+      </c>
+      <c r="C503" s="0" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D503" s="0" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>Acıbadem Alle Bowls</t>
+        </is>
+      </c>
+      <c r="B504" s="1" t="n">
+        <v>44843.04889663649</v>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>Acıbadem Arianas Cheesecake</t>
+        </is>
+      </c>
+      <c r="B505" s="1" t="n">
+        <v>44843.0489639693</v>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>4.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>Acıbadem Big Bold Quick</t>
+        </is>
+      </c>
+      <c r="B506" s="1" t="n">
+        <v>44843.04903370281</v>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>4.3</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>Acıbadem Caesar Salad By</t>
+        </is>
+      </c>
+      <c r="B507" s="1" t="n">
+        <v>44843.04910470795</v>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>Acıbadem Çosa</t>
+        </is>
+      </c>
+      <c r="B508" s="1" t="n">
+        <v>44843.04917422673</v>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>Acıbadem Detroit Bad Boys Pizza</t>
+        </is>
+      </c>
+      <c r="B509" s="1" t="n">
+        <v>44843.04924564865</v>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>Acıbadem Dlycious Dyssert</t>
+        </is>
+      </c>
+      <c r="B510" s="1" t="n">
+        <v>44843.04931850964</v>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>3.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>Acıbadem Doyuyo</t>
+        </is>
+      </c>
+      <c r="B511" s="1" t="n">
+        <v>44843.04938510858</v>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>KAPALI</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>Acıbadem El Pollo Lasso</t>
+        </is>
+      </c>
+      <c r="B512" s="1" t="n">
+        <v>44843.04944940782</v>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>AÇIK</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>4.3</t>
         </is>
       </c>
     </row>

</xml_diff>